<commit_message>
Updated end to end scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Testdata.xlsx
+++ b/src/main/resources/testdata/Testdata.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvenk\eclipse-workspace\com.OrangeHRM\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7C42C5-F575-49C4-AB82-41DFC846150F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B857700-1C61-425C-9796-811692B538B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="SearchProduct" sheetId="2" r:id="rId2"/>
     <sheet name="Category" sheetId="4" r:id="rId3"/>
     <sheet name="AddProduct" sheetId="3" r:id="rId4"/>
+    <sheet name="AddContact" sheetId="5" r:id="rId5"/>
+    <sheet name="EndToEnd" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="92">
   <si>
     <t>Password</t>
   </si>
@@ -205,6 +207,105 @@
   </si>
   <si>
     <t>Video Tutorials</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Alertmsg</t>
+  </si>
+  <si>
+    <t>ajc@testgmail.com</t>
+  </si>
+  <si>
+    <t>testonly</t>
+  </si>
+  <si>
+    <t>Press OK to proceed!</t>
+  </si>
+  <si>
+    <t>Success! Your details have been submitted successfully.</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>testing2</t>
+  </si>
+  <si>
+    <t>testing3</t>
+  </si>
+  <si>
+    <t>testing4</t>
+  </si>
+  <si>
+    <t>testing5</t>
+  </si>
+  <si>
+    <t>successmsg</t>
+  </si>
+  <si>
+    <t>Product1price</t>
+  </si>
+  <si>
+    <t>Product1qty</t>
+  </si>
+  <si>
+    <t>Product2qty</t>
+  </si>
+  <si>
+    <t>Quantitylabel</t>
+  </si>
+  <si>
+    <t>cart_quantity</t>
+  </si>
+  <si>
+    <t>cart_total</t>
+  </si>
+  <si>
+    <t>Totallabel</t>
+  </si>
+  <si>
+    <t>Product1Total</t>
+  </si>
+  <si>
+    <t>Product2Total</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>Pure Cotton V-Neck T-Shirt</t>
+  </si>
+  <si>
+    <t>Rs. 1299</t>
+  </si>
+  <si>
+    <t>Rs. 1799</t>
   </si>
 </sst>
 </file>
@@ -228,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +348,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -261,11 +368,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -549,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -931,7 +1039,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,4 +1269,331 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B325CEFF-1523-4C78-BA1C-0E389FC12ACD}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{98BFF21B-C7B2-46CD-A5CA-62871624CF72}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{BAF61F2F-9174-43C6-9521-E0ABA7F1A190}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{46ADC6E6-2D16-43A5-B478-CD751822CEA2}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{2F5BCA64-FCC4-4713-9588-3F42683F3652}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{CA9B22C5-0CDC-42F7-B2DC-E8159529986E}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{0E088FA0-CF96-44EB-BC3C-F0140CBA69B4}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{B0C28E56-C314-4C76-A952-14306B12E69C}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{D01ED502-9009-4499-8E57-7A24704B7FD2}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{ABF37077-E425-4281-A46C-FC8BFEBB5C83}"/>
+    <hyperlink ref="B5" r:id="rId10" xr:uid="{57A13BA4-FDDD-4B14-937C-B67F96F70552}"/>
+    <hyperlink ref="B6" r:id="rId11" xr:uid="{47C07DFA-2386-4958-B0B8-745004B443B7}"/>
+    <hyperlink ref="D3" r:id="rId12" xr:uid="{90A3DFEE-EDB3-4811-B262-2C01999C4A27}"/>
+    <hyperlink ref="D4" r:id="rId13" xr:uid="{47D7D422-5FF8-493D-A719-128C792C3D64}"/>
+    <hyperlink ref="D5" r:id="rId14" xr:uid="{20AF6DE1-EE0A-417B-B67E-2BE3D79AA06A}"/>
+    <hyperlink ref="D6" r:id="rId15" xr:uid="{5D8127ED-2B0E-4B71-9FB2-523961D87D4D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0AFD68-D520-491C-B9C1-E3ED353B4B72}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" customWidth="1"/>
+    <col min="6" max="6" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="18" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DC4C49EA-6DAC-4E2A-A330-F3BDC5032A7F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{2225DB50-455F-4CB7-8A20-16DED169D040}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed end to end scenario of product checkout
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Testdata.xlsx
+++ b/src/main/resources/testdata/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvenk\eclipse-workspace\com.OrangeHRM\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B857700-1C61-425C-9796-811692B538B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6AD1A7-B87B-43C0-AFFD-3DE306B0958D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="96">
   <si>
     <t>Password</t>
   </si>
@@ -299,13 +299,25 @@
     <t>TotalAmount</t>
   </si>
   <si>
-    <t>Pure Cotton V-Neck T-Shirt</t>
-  </si>
-  <si>
-    <t>Rs. 1299</t>
-  </si>
-  <si>
-    <t>Rs. 1799</t>
+    <t>Rs. 900</t>
+  </si>
+  <si>
+    <t>payeename</t>
+  </si>
+  <si>
+    <t>cardnum</t>
+  </si>
+  <si>
+    <t>cvc</t>
+  </si>
+  <si>
+    <t>monthexpiry</t>
+  </si>
+  <si>
+    <t>yearexpiry</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
@@ -1461,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0AFD68-D520-491C-B9C1-E3ED353B4B72}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1477,7 +1489,7 @@
     <col min="18" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1532,8 +1544,23 @@
       <c r="R1" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1565,16 +1592,16 @@
         <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
         <v>19</v>
@@ -1586,7 +1613,22 @@
         <v>84</v>
       </c>
       <c r="R2" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="S2" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2">
+        <v>12345</v>
+      </c>
+      <c r="U2">
+        <v>311</v>
+      </c>
+      <c r="V2">
+        <v>11</v>
+      </c>
+      <c r="W2">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>